<commit_message>
Completed Multi-Linear Regression Model
Score~ Time + Mark
</commit_message>
<xml_diff>
--- a/Linear Regression Plot/Total Score and Time.xlsx
+++ b/Linear Regression Plot/Total Score and Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Google Drive\R\MIE236-Project\Linear Regression Plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F81FE6D-39FA-4F8E-A151-0C0495E2DF8B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6D66A4-10C6-469F-9D40-B0C751A846BE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11175" xr2:uid="{80DBD79E-4D68-444C-A4DB-1F0FF7B96160}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>M8</t>
   </si>
@@ -82,13 +82,29 @@
   </si>
   <si>
     <t>Student</t>
+  </si>
+  <si>
+    <t>Mark</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -97,7 +113,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -110,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -118,14 +134,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4C6409-D37C-406C-BAD8-079D964FBD14}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -451,7 +489,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -461,8 +499,11 @@
       <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -472,8 +513,11 @@
       <c r="C2" s="1">
         <v>240</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -483,8 +527,11 @@
       <c r="C3" s="1">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -494,8 +541,11 @@
       <c r="C4" s="1">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -505,8 +555,11 @@
       <c r="C5" s="1">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -516,8 +569,11 @@
       <c r="C6" s="1">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -527,8 +583,11 @@
       <c r="C7" s="1">
         <v>143</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -538,8 +597,11 @@
       <c r="C8" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -549,8 +611,11 @@
       <c r="C9" s="1">
         <v>143</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -560,8 +625,11 @@
       <c r="C10" s="1">
         <v>169</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -571,8 +639,11 @@
       <c r="C11" s="1">
         <v>146</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -582,8 +653,11 @@
       <c r="C12" s="1">
         <v>159</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -593,8 +667,11 @@
       <c r="C13" s="1">
         <v>230</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -604,8 +681,11 @@
       <c r="C14" s="1">
         <v>219</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D14" s="4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -615,8 +695,11 @@
       <c r="C15" s="1">
         <v>175</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -626,8 +709,11 @@
       <c r="C16" s="1">
         <v>151</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -636,6 +722,9 @@
       </c>
       <c r="C17" s="1">
         <v>138</v>
+      </c>
+      <c r="D17" s="4">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>